<commit_message>
6.1 Identificación y caracterización de actividades
</commit_message>
<xml_diff>
--- a/estadoDelArte/mapasMentales/referenciasMetodosEvaluaciFRPE/ActividadesYEmocionesCuestionarios.xlsx
+++ b/estadoDelArte/mapasMentales/referenciasMetodosEvaluaciFRPE/ActividadesYEmocionesCuestionarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="89">
   <si>
     <t xml:space="preserve">Actividades</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Poses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcionales</t>
   </si>
   <si>
     <t xml:space="preserve">Interactuar con equipos</t>
@@ -89,6 +92,18 @@
 Emociones</t>
   </si>
   <si>
+    <t xml:space="preserve">Hablar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beber Café</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fumar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Electrónicos</t>
   </si>
   <si>
@@ -101,16 +116,13 @@
     <t xml:space="preserve">Cortés</t>
   </si>
   <si>
-    <t xml:space="preserve">Evasión</t>
+    <t xml:space="preserve">Aislamiento</t>
   </si>
   <si>
     <t xml:space="preserve">Agresivo</t>
   </si>
   <si>
     <t xml:space="preserve">Tembloroso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comer</t>
   </si>
   <si>
     <t xml:space="preserve">Moverse
@@ -1320,17 +1332,29 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Item 1) Dolores en el cuello y espalda o tensión muscular.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Item 1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Dolores en el cuello y espalda o tensión muscular.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1340,17 +1364,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">3. Problemas respiratorios.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Problemas respiratorios.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1360,17 +1396,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">4. Dolor de cabeza.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Dolor de cabeza.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1380,13 +1428,24 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">5. Trastornos del sueño como somnolencia durante el día o</t>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Trastornos del sueño como somnolencia durante el día o</t>
     </r>
     <r>
       <rPr>
@@ -1410,6 +1469,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1419,17 +1479,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10. Dificultad para permanecer quieto o dificultad para iniciar actividades.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Dificultad para permanecer quieto o dificultad para iniciar actividades.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1439,17 +1511,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">11. Dificultad en las relaciones con otras personas .
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Dificultad en las relaciones con otras personas .
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1459,17 +1543,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">12. Sensación de aislamiento y desinterés.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">12)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sensación de aislamiento y desinterés.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1479,17 +1575,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">17. Cansancio, tedio o desgano.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">17)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Cansancio, tedio o desgano.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1499,17 +1607,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">24. Sentimiento de irritabilidad, actitudes y pensamientos negativos.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">24)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sentimiento de irritabilidad, actitudes y pensamientos negativos.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1519,17 +1639,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">25. Sentimiento de angustia, preocupación o tristeza.
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">25)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sentimiento de angustia, preocupación o tristeza.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1539,17 +1671,29 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">28. Consumo de bebidas alcohólicas o café o cigarrillo .
-</t>
-    </r>
-    <r>
-      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">28)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Consumo de bebidas alcohólicas o café o cigarrillo .
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
@@ -1559,26 +1703,248 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">30. Comportamientos rígidos, obstinación o terquedad.</t>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">30)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Comportamientos rígidos, obstinación o terquedad.</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">Cuestionario psicosocial de Copenhague (COPSOQ)</t>
   </si>
   <si>
-    <t xml:space="preserve">5 ¿Tienes que trabajar muy rápido?
-12 ¿Tienes que quedarte después de la hora establecida de salida? 
-26 ¿Tu trabajo requiere que escondas tus emociones?
-29 ¿Tu trabajo requiere atención constante?
-¿Tu puesto de trabajo se encuentra aislado del de tus compañeros o compañeras?
-¿Puedes hablar con tus compañeros o compañeras mientras estás trabajando?
-¿Hay un buen ambiente entre tú y tus compañeros/as de trabajo?</t>
+    <t xml:space="preserve">Copenhagen:
+Arbejdsmiljøinstituttet 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluación y la prevención de los riesgos psicosociales</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Exigencias psicológicas cuantitativas
+Item 5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ¿Tienes que trabajar muy rápido?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Item </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ¿Tienes que quedarte después de la hora establecida de salida? 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Exigencias de esconder emociones
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Item </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">24)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ¿Tu trabajo requiere que escondas tus emociones?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Exigencias psicológicas sensoriales
+Item 25)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ¿Tu trabajo requiere mucha concentración?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Item 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) ¿Tu trabajo requiere atención constante?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Posibilidades de relación social
+Item 81)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ¿Tu puesto de trabajo se encuentra aislado del de tus compañeros o compañeras?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Item 82)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ¿Puedes hablar con tus compañeros o compañeras mientras estás trabajando?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sentimiento de grupo
+Item 83)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ¿Hay un buen ambiente entre tú y tus compañeros/as de trabajo?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1588,7 +1954,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1744,6 +2110,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1937,7 +2310,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1954,6 +2327,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2028,6 +2405,10 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2123,12 +2504,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ13"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AG1" activeCellId="0" sqref="AG1"/>
-      <selection pane="bottomLeft" activeCell="AG13" activeCellId="0" sqref="AG13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2140,26 +2521,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="7.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="0" width="11.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="15.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="0" width="136.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="97.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="37" style="0" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="12" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="24" style="0" width="11.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="10.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="10.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="0" width="11.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="136.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="97.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="10.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="40" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,12 +2559,12 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
+      <c r="Y1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -2193,6 +2572,9 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
@@ -2206,497 +2588,572 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
       <c r="V2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="W2" s="5"/>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="5"/>
+      <c r="Y2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
       <c r="AB2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="K3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="L3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="M3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="N3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="O3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="P3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="Q3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="R3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="S3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="T3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="U3" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="V3" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="W3" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X3" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y3" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z3" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA3" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB3" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AD3" s="16" t="s">
+      <c r="AC3" s="15" t="s">
         <v>40</v>
       </c>
+      <c r="AD3" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="AE3" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AF3" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AH3" s="9" t="s">
+      <c r="AG3" s="17" t="s">
         <v>44</v>
+      </c>
+      <c r="AH3" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA4" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="19" t="s">
+      <c r="A4" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="AH4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="AJ4" s="18"/>
+      <c r="C4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK4" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="AB5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>55</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AE5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ5" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK5" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="S6" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="T6" s="18"/>
-      <c r="AG6" s="19" t="s">
-        <v>59</v>
+      <c r="A6" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="W6" s="19"/>
+      <c r="AJ6" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
-        <v>60</v>
+      <c r="A7" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="T7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="W7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE7" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="AG7" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH7" s="18" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="AH7" s="19"/>
+      <c r="AI7" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ7" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK7" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="111" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
-        <v>64</v>
+      <c r="A8" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="AG8" s="22" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="AJ8" s="23" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG9" s="18"/>
+      <c r="A9" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="T10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="V10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG10" s="19" t="s">
-        <v>72</v>
+      <c r="A10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="W10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ10" s="20" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
-        <v>73</v>
+      <c r="A11" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" s="18"/>
-      <c r="P11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="X11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG11" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R11" s="19"/>
+      <c r="T11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ11" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="152.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG12" s="20" t="s">
-        <v>80</v>
+    <row r="12" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="W12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ12" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="88.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG13" s="20" t="s">
-        <v>82</v>
+    <row r="13" customFormat="false" ht="166.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="19"/>
+      <c r="Q13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ13" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="G1:U1"/>
-    <mergeCell ref="V1:AF1"/>
+  <mergeCells count="11">
+    <mergeCell ref="G1:X1"/>
+    <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AF2:AI2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>

</xml_diff>

<commit_message>
7.2 Artículos detección de Actividades
</commit_message>
<xml_diff>
--- a/estadoDelArte/mapasMentales/referenciasMetodosEvaluaciFRPE/ActividadesYEmocionesCuestionarios.xlsx
+++ b/estadoDelArte/mapasMentales/referenciasMetodosEvaluaciFRPE/ActividadesYEmocionesCuestionarios.xlsx
@@ -9,7 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1_2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="120">
   <si>
     <t xml:space="preserve">Actividades</t>
   </si>
@@ -99,12 +100,6 @@
     <t xml:space="preserve">Llorar</t>
   </si>
   <si>
-    <t xml:space="preserve">Hablar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respirar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ejercitarse</t>
   </si>
   <si>
@@ -139,7 +134,7 @@
 Constantemente</t>
   </si>
   <si>
-    <t xml:space="preserve">Respiración
+    <t xml:space="preserve">Respirar de forma
 Agitada</t>
   </si>
   <si>
@@ -205,7 +200,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 1)</t>
     </r>
@@ -215,7 +209,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> In the last month,</t>
     </r>
@@ -225,7 +218,6 @@
         <color rgb="FF1C3687"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -235,7 +227,6 @@
         <color rgb="FF182F7C"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">how often</t>
     </r>
@@ -245,7 +236,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> have you been</t>
     </r>
@@ -255,7 +245,6 @@
         <color rgb="FFF04E4D"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -265,7 +254,6 @@
         <color rgb="FFBA131A"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">upset</t>
     </r>
@@ -275,7 +263,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> because of something that happened unexpectedly?
 </t>
@@ -287,7 +274,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 3)</t>
     </r>
@@ -297,7 +283,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> In the last month, how often have you felt nervous and “stressed”?
 </t>
@@ -309,7 +294,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 7)</t>
     </r>
@@ -319,7 +303,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> In the last month, </t>
     </r>
@@ -329,7 +312,6 @@
         <color rgb="FF182F7C"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">how often</t>
     </r>
@@ -339,7 +321,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> have you been </t>
     </r>
@@ -349,7 +330,6 @@
         <color rgb="FF00864B"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">able to control</t>
     </r>
@@ -359,7 +339,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -369,7 +348,6 @@
         <color rgb="FFBA131A"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">irritations </t>
     </r>
@@ -379,7 +357,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">in your life?
 </t>
@@ -391,7 +368,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 9)</t>
     </r>
@@ -401,7 +377,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> In the last month,</t>
     </r>
@@ -411,7 +386,6 @@
         <color rgb="FF182F7C"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> how often</t>
     </r>
@@ -421,7 +395,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> have you been </t>
     </r>
@@ -431,7 +404,6 @@
         <color rgb="FFBA131A"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">angered</t>
     </r>
@@ -441,7 +413,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> because of things that were outside of your control?</t>
     </r>
@@ -482,7 +453,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 4 a )</t>
     </r>
@@ -492,7 +462,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> I experienced breathing difficulty (e.g. excessively rapid breathing, breathlessness in the absence of physical exertion)
 </t>
@@ -504,7 +473,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 7 a )</t>
     </r>
@@ -514,7 +482,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> I experienced trembling (e.g. in the hands)
 </t>
@@ -526,7 +493,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 11 s )</t>
     </r>
@@ -536,7 +502,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> I found myself getting agitated
 </t>
@@ -548,7 +513,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 12 s )</t>
     </r>
@@ -558,7 +522,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> I found it difficult to relax
 </t>
@@ -570,7 +533,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 13 d )</t>
     </r>
@@ -580,7 +542,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> I felt down-hearted and blue
 </t>
@@ -592,7 +553,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 16 d )</t>
     </r>
@@ -602,7 +562,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -612,7 +571,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">I was unable to become enthusiastic about anything
 </t>
@@ -624,7 +582,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 20 a )</t>
     </r>
@@ -634,7 +591,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -644,7 +600,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">I felt scared without any good reason</t>
     </r>
@@ -663,7 +618,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Albert J. Stunkard and Samuel Messick, </t>
     </r>
@@ -673,7 +627,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1985</t>
     </r>
@@ -692,7 +645,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 3)</t>
     </r>
@@ -702,7 +654,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> When I feel anxious, I find myself eating.
 </t>
@@ -714,7 +665,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 4)</t>
     </r>
@@ -724,7 +674,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Sometimes when I start eating, I just can’t seem to stop
 </t>
@@ -736,7 +685,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 6)</t>
     </r>
@@ -746,7 +694,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> When I feel blue, I often overeat.
 </t>
@@ -758,7 +705,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 14)</t>
     </r>
@@ -768,7 +714,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> How often do you feel hungry?</t>
     </r>
@@ -794,7 +739,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 1)</t>
     </r>
@@ -804,7 +748,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the last 30 days, about how often did you feel tired out for no good reason?
 </t>
@@ -816,7 +759,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 2)</t>
     </r>
@@ -826,7 +768,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the last 30 days, about how often did you feel nervous?
 </t>
@@ -838,7 +779,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 3)</t>
     </r>
@@ -848,7 +788,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the last 30 days, about how often did you feel so nervous that nothing could calm you Down?
 </t>
@@ -860,7 +799,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 5)</t>
     </r>
@@ -870,7 +808,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the last 30 days, about how often did you feel restless or fidgety?
 </t>
@@ -882,7 +819,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 6)</t>
     </r>
@@ -892,7 +828,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the last 30 days, about how often did you feel so restless you could not sit still?
 </t>
@@ -904,7 +839,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 7)</t>
     </r>
@@ -914,7 +848,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the last 30 days, about how often did you feel depressed?
 </t>
@@ -926,7 +859,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 9)</t>
     </r>
@@ -936,7 +868,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the last 30 days, about how often did you feel so sad that nothing could cheer you up?</t>
     </r>
@@ -971,7 +902,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 7) </t>
     </r>
@@ -981,7 +911,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">During the past month, how often have you had trouble staying awake while driving, eating meals, or engaging in social activity?</t>
     </r>
@@ -1003,7 +932,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Aerobic Excercise
 </t>
@@ -1014,7 +942,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 1) In the past month, how often did you engage in aerobic exercise?
 Item 2) In the past month, what is the average number of days per week that you engaged in aerobic exercise?
@@ -1028,7 +955,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tobbaco Use
 Item 4) </t>
@@ -1039,7 +965,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">How would you describe your smoking during your last year in high school?
 </t>
@@ -1051,7 +976,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 5)</t>
     </r>
@@ -1061,7 +985,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> During the past month, how many cigarettes have you smoked on an average day?
 </t>
@@ -1073,7 +996,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 8)</t>
     </r>
@@ -1083,7 +1005,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> In the past month, were there times when you tried to cut back or quit smoking?
 In the past month, have you :
@@ -1098,7 +1019,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 13)</t>
     </r>
@@ -1108,7 +1028,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> In the past month, about how many times did you actually get drunk?
 Eating
@@ -1121,7 +1040,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 2) </t>
     </r>
@@ -1131,7 +1049,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Do you usually snack instead of eating regular meals?</t>
     </r>
@@ -1158,7 +1075,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 12) </t>
     </r>
@@ -1168,7 +1084,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Me siento con mucha energía en mi trabajo.
 </t>
@@ -1180,7 +1095,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 14) </t>
     </r>
@@ -1190,7 +1104,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Creo que trabajo demasiado.
 </t>
@@ -1202,7 +1115,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 16)</t>
     </r>
@@ -1212,7 +1124,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Trabajar directamente con alumnos/as me produce estrés.
 </t>
@@ -1224,7 +1135,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 18)</t>
     </r>
@@ -1234,7 +1144,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Me siento motivado después de trabajar en contacto con alumnos/as.</t>
     </r>
@@ -1256,7 +1165,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 7) </t>
     </r>
@@ -1266,7 +1174,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Me cuesta mucho ser cortés con los usuarios de mi trabajo.
 </t>
@@ -1278,7 +1185,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 10)</t>
     </r>
@@ -1288,7 +1194,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Hace mucho tiempo que dejé de hacer mi trabajo con pasión.
 </t>
@@ -1300,7 +1205,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 14) Las situaciones a las que me enfrento en mi trabajo no me provocan tensión alguna.
 Item 16)</t>
@@ -1311,7 +1215,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> En mi trabajo todos me parecen extraños, por lo cual no me interesa interactuar con ellos.
 </t>
@@ -1323,7 +1226,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 23)</t>
     </r>
@@ -1333,7 +1235,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Aunque un usuario de mi trabajo sea descortés conmigo, lo trato bien.
 </t>
@@ -1345,7 +1246,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 32)</t>
     </r>
@@ -1355,7 +1255,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Te sientes deprimido (muy triste).
 </t>
@@ -1367,7 +1266,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 34) </t>
     </r>
@@ -1377,7 +1275,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tienes dolores de cabeza.
 </t>
@@ -1389,7 +1286,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 41)</t>
     </r>
@@ -1399,7 +1295,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Te sientes desesperado (ansioso).
 </t>
@@ -1411,7 +1306,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 43)</t>
     </r>
@@ -1421,7 +1315,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Te duelen las articulaciones de brazos y piernas.
 </t>
@@ -1433,7 +1326,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 47)</t>
     </r>
@@ -1443,7 +1335,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Tienes dolores en el abdomen.
 </t>
@@ -1455,7 +1346,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 49)</t>
     </r>
@@ -1465,7 +1355,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Te duele la espalda y el cuello
 </t>
@@ -1477,7 +1366,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 59)</t>
     </r>
@@ -1487,7 +1375,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Te duele el pecho.
 </t>
@@ -1519,7 +1406,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 1)</t>
     </r>
@@ -1529,7 +1415,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Dolores en el cuello y espalda o tensión muscular.
 </t>
@@ -1541,7 +1426,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 3)</t>
     </r>
@@ -1551,7 +1435,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Problemas respiratorios.
 </t>
@@ -1563,7 +1446,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 4)</t>
     </r>
@@ -1573,7 +1455,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Dolor de cabeza.
 </t>
@@ -1585,7 +1466,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 5)</t>
     </r>
@@ -1595,7 +1475,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Trastornos del sueño como somnolencia durante el día o desvelo en la noche.
 </t>
@@ -1607,7 +1486,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 10)</t>
     </r>
@@ -1617,7 +1495,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Dificultad para permanecer quieto o dificultad para iniciar actividades.
 </t>
@@ -1629,7 +1506,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 11)</t>
     </r>
@@ -1639,7 +1515,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Dificultad en las relaciones con otras personas .
 </t>
@@ -1651,7 +1526,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 12)</t>
     </r>
@@ -1661,7 +1535,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Sensación de aislamiento y desinterés.
 </t>
@@ -1673,7 +1546,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 17)</t>
     </r>
@@ -1683,7 +1555,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Cansancio, tedio o desgano.
 </t>
@@ -1695,7 +1566,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 24)</t>
     </r>
@@ -1705,7 +1575,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Sentimiento de irritabilidad, actitudes y pensamientos negativos.
 </t>
@@ -1717,7 +1586,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 25)</t>
     </r>
@@ -1727,7 +1595,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Sentimiento de angustia, preocupación o tristeza.
 </t>
@@ -1739,7 +1606,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 28)</t>
     </r>
@@ -1749,7 +1615,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Consumo de bebidas alcohólicas o café o cigarrillo .
 </t>
@@ -1761,7 +1626,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 30)</t>
     </r>
@@ -1771,7 +1635,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Comportamientos rígidos, obstinación o terquedad.</t>
     </r>
@@ -1797,7 +1660,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Exigencias psicológicas cuantitativas
 Item 5)</t>
@@ -1808,7 +1670,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ¿Tienes que trabajar muy rápido?
 </t>
@@ -1820,7 +1681,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 11)</t>
     </r>
@@ -1830,7 +1690,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ¿Tienes que quedarte después de la hora establecida de salida? 
 </t>
@@ -1842,7 +1701,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Exigencias de esconder emociones
 Item 24)</t>
@@ -1853,7 +1711,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ¿Tu trabajo requiere que escondas tus emociones?
 </t>
@@ -1865,7 +1722,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Exigencias psicológicas sensoriales
 Item 25)</t>
@@ -1876,7 +1732,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ¿Tu trabajo requiere mucha concentración?
 </t>
@@ -1888,7 +1743,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 27</t>
     </r>
@@ -1898,7 +1752,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">) ¿Tu trabajo requiere atención constante?
 </t>
@@ -1910,7 +1763,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Posibilidades de relación social
 Item 81)</t>
@@ -1921,7 +1773,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ¿Tu puesto de trabajo se encuentra aislado del de tus compañeros o compañeras?
 </t>
@@ -1933,7 +1784,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Item 82)</t>
     </r>
@@ -1943,7 +1793,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ¿Puedes hablar con tus compañeros o compañeras mientras estás trabajando?
 </t>
@@ -1955,7 +1804,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Sentimiento de grupo
 Item 83)</t>
@@ -1966,7 +1814,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ¿Hay un buen ambiente entre tú y tus compañeros/as de trabajo?</t>
     </r>
@@ -1992,7 +1839,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1. Sadness
 </t>
@@ -2003,7 +1849,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0. I do not feel sad.
 1. I feel sad much of the time.
@@ -2018,7 +1863,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10. Crying
 </t>
@@ -2029,7 +1873,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0. I don't cry anymore than I used to.
 1. I cry more than I used to.
@@ -2044,7 +1887,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">11. Agitation
 </t>
@@ -2055,7 +1897,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0. I am no more restless or wound up than usual.
 1. I feel more restless or wound up than usual.
@@ -2071,7 +1912,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">12. Loss of Interest
 </t>
@@ -2082,7 +1922,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0. I have not lost interest in other people or
 activities.
@@ -2100,7 +1939,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">17. Irritability
 </t>
@@ -2111,7 +1949,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0. I am not more irritable than usual.
 1. I am more irritable than usual.
@@ -2126,7 +1963,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">18. Changes in Appetite
 </t>
@@ -2137,7 +1973,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0. I have not experienced any change in my appetite.
 1a My appetite is somewhat less than usual.
@@ -2180,6 +2015,12 @@
   </si>
   <si>
     <t xml:space="preserve">Requiere imágenes de alta resolución (720p-1080p)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hablar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respirar</t>
   </si>
 </sst>
 </file>
@@ -2189,13 +2030,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2214,11 +2054,87 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2226,72 +2142,98 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1C3687"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF182F7C"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFF04E4D"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFBA131A"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00864B"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFBA131A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF7477B8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFBEE3D3"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2314,7 +2256,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBEE3D3"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -2336,12 +2278,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -2352,7 +2309,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2376,105 +2333,152 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2482,69 +2486,90 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF00864B"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFBEE3D3"/>
       <rgbColor rgb="FF390A5D"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -2555,12 +2580,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFBEE3D3"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFF7A19A"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -2587,12 +2612,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ33"/>
+  <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AN3" activeCellId="0" sqref="AN3:AO3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2604,7 +2627,1283 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="3.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="14" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="5.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="6.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="30" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="34" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="38" style="0" width="136.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="97.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="41" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="10.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="103.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH3" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL3" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM3" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="27.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM4" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="28.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="22"/>
+      <c r="AK5" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL5" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL6" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD7" s="26"/>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH7" s="26"/>
+      <c r="AI7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL7" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM7" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="31.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="26"/>
+      <c r="AH8" s="26"/>
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="S9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH9" s="26"/>
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="U10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" s="26"/>
+      <c r="AA10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB10" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="26"/>
+      <c r="AG10" s="26"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="26"/>
+      <c r="AK10" s="26"/>
+      <c r="AL10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="38.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="W11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD11" s="26"/>
+      <c r="AE11" s="26"/>
+      <c r="AF11" s="26"/>
+      <c r="AG11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH11" s="26"/>
+      <c r="AI11" s="26"/>
+      <c r="AJ11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK11" s="26"/>
+      <c r="AL11" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="W12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL12" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="62.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB13" s="22"/>
+      <c r="AC13" s="26"/>
+      <c r="AD13" s="26"/>
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="26"/>
+      <c r="AL13" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="31.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="22"/>
+      <c r="AB14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC14" s="26"/>
+      <c r="AD14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="26"/>
+      <c r="AK14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL14" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="62.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="21"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="22"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="22"/>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26"/>
+      <c r="AI15" s="26"/>
+      <c r="AJ15" s="26"/>
+      <c r="AK15" s="26"/>
+      <c r="AL15" s="30"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="32"/>
+      <c r="AB16" s="32"/>
+      <c r="AC16" s="32"/>
+      <c r="AD16" s="32"/>
+      <c r="AE16" s="32"/>
+      <c r="AF16" s="32"/>
+      <c r="AG16" s="32"/>
+      <c r="AH16" s="32"/>
+      <c r="AI16" s="32"/>
+      <c r="AJ16" s="32"/>
+      <c r="AK16" s="32"/>
+      <c r="AL16" s="32"/>
+      <c r="AM16" s="32"/>
+      <c r="AN16" s="1"/>
+    </row>
+    <row r="17" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="32"/>
+      <c r="AB17" s="32"/>
+      <c r="AC17" s="32"/>
+      <c r="AD17" s="32"/>
+      <c r="AE17" s="32"/>
+      <c r="AF17" s="32"/>
+      <c r="AG17" s="32"/>
+      <c r="AH17" s="32"/>
+      <c r="AI17" s="32"/>
+      <c r="AJ17" s="32"/>
+      <c r="AK17" s="32"/>
+      <c r="AL17" s="32"/>
+      <c r="AM17" s="32"/>
+      <c r="AMI17" s="0"/>
+      <c r="AMJ17" s="0"/>
+    </row>
+    <row r="18" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AMI18" s="0"/>
+      <c r="AMJ18" s="0"/>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AMI19" s="0"/>
+      <c r="AMJ19" s="0"/>
+    </row>
+    <row r="20" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AMI20" s="0"/>
+      <c r="AMJ20" s="0"/>
+    </row>
+    <row r="21" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AMI21" s="0"/>
+      <c r="AMJ21" s="0"/>
+    </row>
+    <row r="22" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AMI22" s="0"/>
+      <c r="AMJ22" s="0"/>
+    </row>
+    <row r="23" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AMI23" s="0"/>
+      <c r="AMJ23" s="0"/>
+    </row>
+    <row r="24" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI24" s="0"/>
+      <c r="AMJ24" s="0"/>
+    </row>
+    <row r="25" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI25" s="0"/>
+      <c r="AMJ25" s="0"/>
+    </row>
+    <row r="26" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="AMI26" s="0"/>
+      <c r="AMJ26" s="0"/>
+    </row>
+    <row r="27" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AMI27" s="0"/>
+      <c r="AMJ27" s="0"/>
+    </row>
+    <row r="28" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AMI28" s="0"/>
+      <c r="AMJ28" s="0"/>
+    </row>
+    <row r="29" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AMI29" s="0"/>
+      <c r="AMJ29" s="0"/>
+    </row>
+    <row r="30" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI30" s="0"/>
+      <c r="AMJ30" s="0"/>
+    </row>
+    <row r="31" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI31" s="0"/>
+      <c r="AMJ31" s="0"/>
+    </row>
+    <row r="32" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI32" s="0"/>
+      <c r="AMJ32" s="0"/>
+    </row>
+    <row r="33" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMI33" s="0"/>
+      <c r="AMJ33" s="0"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="H1:Z1"/>
+    <mergeCell ref="AA1:AK1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AH2:AK2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AQ33"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="14" style="0" width="3.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="5.75"/>
@@ -2615,8 +3914,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="36" style="0" width="3.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="40" style="0" width="136.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="97.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="44" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="43" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,123 +4075,123 @@
         <v>24</v>
       </c>
       <c r="O3" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="T3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="U3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="V3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="Z3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="AA3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="AB3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AA3" s="14" t="s">
+      <c r="AC3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AB3" s="14" t="s">
+      <c r="AD3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AC3" s="15" t="s">
+      <c r="AE3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AF3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AE3" s="15" t="s">
+      <c r="AG3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="AF3" s="16" t="s">
+      <c r="AH3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AI3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AH3" s="16" t="s">
+      <c r="AJ3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="AI3" s="17" t="s">
+      <c r="AK3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="AJ3" s="18" t="s">
+      <c r="AL3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="AK3" s="18" t="s">
+      <c r="AM3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="AL3" s="18" t="s">
+      <c r="AN3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="AM3" s="19" t="s">
+      <c r="AO3" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="AN3" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="AO3" s="20" t="s">
-        <v>51</v>
       </c>
       <c r="AP3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="27.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="D4" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>55</v>
-      </c>
       <c r="E4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
       <c r="M4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
-      <c r="P4" s="23"/>
+      <c r="P4" s="26"/>
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
@@ -2910,199 +4208,199 @@
       <c r="AD4" s="22"/>
       <c r="AE4" s="22"/>
       <c r="AF4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AG4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AH4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AI4" s="22"/>
       <c r="AJ4" s="22"/>
       <c r="AK4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AL4" s="22"/>
       <c r="AM4" s="22"/>
-      <c r="AN4" s="24" t="s">
-        <v>57</v>
+      <c r="AN4" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="AO4" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="25"/>
+      <c r="AQ4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="28.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="D5" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>62</v>
-      </c>
       <c r="E5" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
       <c r="P5" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
       <c r="Z5" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AA5" s="22"/>
       <c r="AB5" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AC5" s="22"/>
       <c r="AD5" s="22"/>
       <c r="AE5" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="26"/>
       <c r="AI5" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ5" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK5" s="22"/>
       <c r="AL5" s="22"/>
-      <c r="AM5" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN5" s="24" t="s">
-        <v>63</v>
+      <c r="AM5" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN5" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="AO5" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AP5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="D6" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="E6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="26"/>
+      <c r="AI6" s="26"/>
+      <c r="AJ6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN6" s="23" t="s">
         <v>67</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="23"/>
-      <c r="AG6" s="23"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="23"/>
-      <c r="AJ6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM6" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN6" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="AO6" s="5"/>
       <c r="AP6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>73</v>
-      </c>
       <c r="E7" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="G7" s="26"/>
       <c r="H7" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
@@ -3120,75 +4418,75 @@
       <c r="W7" s="22"/>
       <c r="X7" s="22"/>
       <c r="Y7" s="22"/>
-      <c r="Z7" s="23"/>
+      <c r="Z7" s="26"/>
       <c r="AA7" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="26"/>
       <c r="AE7" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="23"/>
-      <c r="AH7" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="26"/>
+      <c r="AH7" s="26"/>
       <c r="AI7" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ7" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AJ7" s="26"/>
       <c r="AK7" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AL7" s="22"/>
       <c r="AM7" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN7" s="24" t="s">
-        <v>74</v>
+        <v>54</v>
+      </c>
+      <c r="AN7" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="AO7" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AP7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="31.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="D8" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>79</v>
-      </c>
       <c r="E8" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="G8" s="26"/>
       <c r="H8" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K8" s="22"/>
       <c r="L8" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
@@ -3198,452 +4496,452 @@
       <c r="U8" s="22"/>
       <c r="V8" s="22"/>
       <c r="W8" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X8" s="22"/>
       <c r="Y8" s="22"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
-      <c r="AH8" s="23"/>
-      <c r="AI8" s="23"/>
-      <c r="AJ8" s="23"/>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="23"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="26"/>
+      <c r="AH8" s="26"/>
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="26"/>
+      <c r="AM8" s="26"/>
       <c r="AN8" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AO8" s="5"/>
       <c r="AP8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
       <c r="Q9" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="R9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="S9" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="S9" s="26"/>
       <c r="T9" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
-      <c r="AH9" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
+      <c r="AH9" s="26"/>
       <c r="AI9" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="23"/>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="24" t="s">
-        <v>84</v>
+        <v>54</v>
+      </c>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26"/>
+      <c r="AM9" s="26"/>
+      <c r="AN9" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="AO9" s="5"/>
       <c r="AP9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="D10" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>88</v>
-      </c>
       <c r="E10" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
       <c r="V10" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="W10" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X10" s="22"/>
       <c r="Y10" s="22"/>
-      <c r="Z10" s="23"/>
+      <c r="Z10" s="26"/>
       <c r="AA10" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB10" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AB10" s="26"/>
       <c r="AC10" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AD10" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE10" s="23"/>
-      <c r="AF10" s="23"/>
-      <c r="AG10" s="23"/>
-      <c r="AH10" s="23"/>
-      <c r="AI10" s="23"/>
-      <c r="AJ10" s="23"/>
-      <c r="AK10" s="23"/>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="24" t="s">
-        <v>89</v>
+        <v>54</v>
+      </c>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="26"/>
+      <c r="AG10" s="26"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="26"/>
+      <c r="AK10" s="26"/>
+      <c r="AL10" s="26"/>
+      <c r="AM10" s="26"/>
+      <c r="AN10" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="AO10" s="5"/>
       <c r="AP10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="38.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="E11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
       <c r="K11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
       <c r="W11" s="22"/>
       <c r="X11" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Y11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="26"/>
+      <c r="AD11" s="26"/>
       <c r="AE11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AF11" s="26"/>
+      <c r="AG11" s="26"/>
+      <c r="AH11" s="26"/>
       <c r="AI11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ11" s="23"/>
-      <c r="AK11" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AJ11" s="26"/>
+      <c r="AK11" s="26"/>
       <c r="AL11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM11" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AM11" s="26"/>
       <c r="AN11" s="30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AO11" s="5"/>
       <c r="AP11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="34.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="D12" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>97</v>
-      </c>
       <c r="E12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
       <c r="J12" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
       <c r="S12" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="T12" s="22"/>
       <c r="U12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
       <c r="X12" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Y12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z12" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="Z12" s="26"/>
       <c r="AA12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="23"/>
-      <c r="AD12" s="23"/>
-      <c r="AE12" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="26"/>
       <c r="AF12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG12" s="23"/>
-      <c r="AH12" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="26"/>
       <c r="AI12" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ12" s="23"/>
-      <c r="AK12" s="23"/>
-      <c r="AL12" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="26"/>
+      <c r="AL12" s="26"/>
       <c r="AM12" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AN12" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AO12" s="5"/>
       <c r="AP12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="62.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="D13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>102</v>
-      </c>
       <c r="E13" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
       <c r="M13" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
       <c r="X13" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
       <c r="AC13" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AD13" s="22"/>
-      <c r="AE13" s="23"/>
-      <c r="AF13" s="23"/>
-      <c r="AG13" s="23"/>
-      <c r="AH13" s="23"/>
-      <c r="AI13" s="23"/>
-      <c r="AJ13" s="23"/>
-      <c r="AK13" s="23"/>
-      <c r="AL13" s="23"/>
-      <c r="AM13" s="23"/>
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="26"/>
+      <c r="AL13" s="26"/>
+      <c r="AM13" s="26"/>
       <c r="AN13" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AO13" s="5"/>
       <c r="AP13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="31.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="D14" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>107</v>
-      </c>
       <c r="E14" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
       <c r="J14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
-      <c r="S14" s="23"/>
+      <c r="S14" s="26"/>
       <c r="T14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
       <c r="X14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
       <c r="AA14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AB14" s="26"/>
       <c r="AC14" s="22"/>
       <c r="AD14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AE14" s="26"/>
       <c r="AF14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG14" s="23"/>
-      <c r="AH14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
       <c r="AI14" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ14" s="23"/>
-      <c r="AK14" s="23"/>
-      <c r="AL14" s="23"/>
+        <v>54</v>
+      </c>
+      <c r="AJ14" s="26"/>
+      <c r="AK14" s="26"/>
+      <c r="AL14" s="26"/>
       <c r="AM14" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AN14" s="30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AO14" s="5"/>
       <c r="AP14" s="1"/>
@@ -3656,38 +4954,38 @@
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
       <c r="X15" s="22"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
       <c r="AC15" s="22"/>
       <c r="AD15" s="22"/>
-      <c r="AE15" s="23"/>
-      <c r="AF15" s="23"/>
-      <c r="AG15" s="23"/>
-      <c r="AH15" s="23"/>
-      <c r="AI15" s="23"/>
-      <c r="AJ15" s="23"/>
-      <c r="AK15" s="23"/>
-      <c r="AL15" s="23"/>
-      <c r="AM15" s="23"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26"/>
+      <c r="AI15" s="26"/>
+      <c r="AJ15" s="26"/>
+      <c r="AK15" s="26"/>
+      <c r="AL15" s="26"/>
+      <c r="AM15" s="26"/>
       <c r="AN15" s="30"/>
       <c r="AO15" s="5"/>
       <c r="AP15" s="1"/>
@@ -3738,7 +5036,7 @@
     </row>
     <row r="17" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -3783,54 +5081,54 @@
     </row>
     <row r="18" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3860,15 +5158,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AN3:AO3 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>